<commit_message>
completed SVM task but weird output
</commit_message>
<xml_diff>
--- a/test_tsm.xlsx
+++ b/test_tsm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sook Mun\Google Drive\Y3S2\CS2\fit3162\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91C936D2-A8CB-44E2-B450-883F348D04A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B5764A-5016-4996-A9BE-FE2677E6B98B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1530" yWindow="7935" windowWidth="23580" windowHeight="11805" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="23580" windowHeight="11805" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
   <si>
     <t>N</t>
   </si>
   <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>Contrast</t>
+  </si>
+  <si>
+    <t>Correlation</t>
+  </si>
+  <si>
+    <t>Energy</t>
+  </si>
+  <si>
+    <t>Homogeneity</t>
+  </si>
+  <si>
+    <t>Actual Condition</t>
   </si>
 </sst>
 </file>
@@ -348,77 +363,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>4.257884874666636E-3</v>
-      </c>
-      <c r="B1">
-        <v>0.98827356423118484</v>
-      </c>
-      <c r="C1">
-        <v>0.63265887626159634</v>
-      </c>
-      <c r="D1">
-        <v>0.99787105756266681</v>
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>7.7838263440382447E-3</v>
+        <v>4.8273865320502349E-3</v>
       </c>
       <c r="B2">
-        <v>0.97134155129533339</v>
+        <v>0.98370859287657608</v>
       </c>
       <c r="C2">
-        <v>0.72067007332427313</v>
+        <v>0.69888102575816557</v>
       </c>
       <c r="D2">
-        <v>0.99610808682798102</v>
+        <v>0.99758630673397475</v>
       </c>
       <c r="E2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>5.8154145752291626E-3</v>
+        <v>1.0702044568282389E-2</v>
       </c>
       <c r="B3">
-        <v>0.96610384167052643</v>
+        <v>0.94416163197763725</v>
       </c>
       <c r="C3">
-        <v>0.82265280937649032</v>
+        <v>0.79775136177281991</v>
       </c>
       <c r="D3">
-        <v>0.99709229271238553</v>
+        <v>0.99464897771585892</v>
       </c>
       <c r="E3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3.6874276775894408E-3</v>
+        <v>5.9186128621375993E-3</v>
       </c>
       <c r="B4">
-        <v>0.97758081914203265</v>
+        <v>0.98258193315077647</v>
       </c>
       <c r="C4">
-        <v>0.83184970168536321</v>
+        <v>0.65431907259035682</v>
       </c>
       <c r="D4">
-        <v>0.99815628616120533</v>
+        <v>0.99704069356893121</v>
       </c>
       <c r="E4" t="s">
         <v>1</v>
@@ -426,16 +441,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2.6888886977809502E-3</v>
+        <v>4.257884874666636E-3</v>
       </c>
       <c r="B5">
-        <v>0.98317313890742608</v>
+        <v>0.98827356423118484</v>
       </c>
       <c r="C5">
-        <v>0.83752093874877975</v>
+        <v>0.63265887626159634</v>
       </c>
       <c r="D5">
-        <v>0.99865555565110964</v>
+        <v>0.99787105756266681</v>
       </c>
       <c r="E5" t="s">
         <v>0</v>
@@ -443,16 +458,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>9.2467576149347034E-3</v>
+        <v>7.7838263440382447E-3</v>
       </c>
       <c r="B6">
-        <v>0.97445361364154626</v>
+        <v>0.97134155129533339</v>
       </c>
       <c r="C6">
-        <v>0.62887922996523227</v>
+        <v>0.72067007332427313</v>
       </c>
       <c r="D6">
-        <v>0.99537662119253267</v>
+        <v>0.99610808682798102</v>
       </c>
       <c r="E6" t="s">
         <v>1</v>
@@ -460,18 +475,86 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
+        <v>5.8154145752291626E-3</v>
+      </c>
+      <c r="B7">
+        <v>0.96610384167052643</v>
+      </c>
+      <c r="C7">
+        <v>0.82265280937649032</v>
+      </c>
+      <c r="D7">
+        <v>0.99709229271238553</v>
+      </c>
+      <c r="E7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3.6874276775894408E-3</v>
+      </c>
+      <c r="B8">
+        <v>0.97758081914203265</v>
+      </c>
+      <c r="C8">
+        <v>0.83184970168536321</v>
+      </c>
+      <c r="D8">
+        <v>0.99815628616120533</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2.6888886977809502E-3</v>
+      </c>
+      <c r="B9">
+        <v>0.98317313890742608</v>
+      </c>
+      <c r="C9">
+        <v>0.83752093874877975</v>
+      </c>
+      <c r="D9">
+        <v>0.99865555565110964</v>
+      </c>
+      <c r="E9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9.2467576149347034E-3</v>
+      </c>
+      <c r="B10">
+        <v>0.97445361364154626</v>
+      </c>
+      <c r="C10">
+        <v>0.62887922996523227</v>
+      </c>
+      <c r="D10">
+        <v>0.99537662119253267</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>1.4939863109383495E-2</v>
       </c>
-      <c r="B7">
+      <c r="B11">
         <v>0.95996008200223248</v>
       </c>
-      <c r="C7">
+      <c r="C11">
         <v>0.6121591179587238</v>
       </c>
-      <c r="D7">
+      <c r="D11">
         <v>0.99253006844530833</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E11" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
SVM files after running more images
</commit_message>
<xml_diff>
--- a/test_tsm.xlsx
+++ b/test_tsm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sook Mun\Google Drive\Y3S2\CS2\fit3162\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B5764A-5016-4996-A9BE-FE2677E6B98B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEF514BA-164F-4A23-BCFE-263164174D05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="23580" windowHeight="11805" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4335" yWindow="1965" windowWidth="23580" windowHeight="11805" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,22 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="9">
+  <si>
+    <t>Contrast</t>
+  </si>
+  <si>
+    <t>Correlation</t>
+  </si>
+  <si>
+    <t>Energy</t>
+  </si>
+  <si>
+    <t>Homogeneity</t>
+  </si>
+  <si>
+    <t>Actual Condition</t>
+  </si>
   <si>
     <t>N</t>
   </si>
@@ -33,19 +48,10 @@
     <t>B</t>
   </si>
   <si>
-    <t>Contrast</t>
-  </si>
-  <si>
-    <t>Correlation</t>
-  </si>
-  <si>
-    <t>Energy</t>
-  </si>
-  <si>
-    <t>Homogeneity</t>
-  </si>
-  <si>
-    <t>Actual Condition</t>
+    <t>SVM Output</t>
+  </si>
+  <si>
+    <t>'N'</t>
   </si>
 </sst>
 </file>
@@ -363,32 +369,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="19.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>4.8273865320502349E-3</v>
       </c>
@@ -402,10 +414,13 @@
         <v>0.99758630673397475</v>
       </c>
       <c r="E2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1.0702044568282389E-2</v>
       </c>
@@ -419,10 +434,13 @@
         <v>0.99464897771585892</v>
       </c>
       <c r="E3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5.9186128621375993E-3</v>
       </c>
@@ -436,10 +454,13 @@
         <v>0.99704069356893121</v>
       </c>
       <c r="E4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4.257884874666636E-3</v>
       </c>
@@ -453,10 +474,13 @@
         <v>0.99787105756266681</v>
       </c>
       <c r="E5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>7.7838263440382447E-3</v>
       </c>
@@ -470,10 +494,13 @@
         <v>0.99610808682798102</v>
       </c>
       <c r="E6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="F6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5.8154145752291626E-3</v>
       </c>
@@ -487,10 +514,13 @@
         <v>0.99709229271238553</v>
       </c>
       <c r="E7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="F7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3.6874276775894408E-3</v>
       </c>
@@ -504,10 +534,13 @@
         <v>0.99815628616120533</v>
       </c>
       <c r="E8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="F8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2.6888886977809502E-3</v>
       </c>
@@ -521,10 +554,13 @@
         <v>0.99865555565110964</v>
       </c>
       <c r="E9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="F9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9.2467576149347034E-3</v>
       </c>
@@ -538,10 +574,13 @@
         <v>0.99537662119253267</v>
       </c>
       <c r="E10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="F10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1.4939863109383495E-2</v>
       </c>
@@ -555,7 +594,10 @@
         <v>0.99253006844530833</v>
       </c>
       <c r="E11" t="s">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="F11" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>